<commit_message>
Updated real config file letters.xlsx
</commit_message>
<xml_diff>
--- a/model/letters.xlsx
+++ b/model/letters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>א</t>
   </si>
@@ -128,13 +128,94 @@
     <t>letters</t>
   </si>
   <si>
-    <t>jk</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>re</t>
+    <t>nikud</t>
+  </si>
+  <si>
+    <t>ֱ</t>
+  </si>
+  <si>
+    <t>ִ</t>
+  </si>
+  <si>
+    <t>ֵ</t>
+  </si>
+  <si>
+    <t>ֶ</t>
+  </si>
+  <si>
+    <t>ַ</t>
+  </si>
+  <si>
+    <t>ָ</t>
+  </si>
+  <si>
+    <t>ֲ</t>
+  </si>
+  <si>
+    <t>ֳ</t>
+  </si>
+  <si>
+    <t>ׂ</t>
+  </si>
+  <si>
+    <t>ׁ</t>
+  </si>
+  <si>
+    <t>ֹ</t>
+  </si>
+  <si>
+    <t>ּ</t>
+  </si>
+  <si>
+    <t>ֱּ</t>
+  </si>
+  <si>
+    <t>ֲּ</t>
+  </si>
+  <si>
+    <t>ֳּ</t>
+  </si>
+  <si>
+    <t>ִּ</t>
+  </si>
+  <si>
+    <t>ֵּ</t>
+  </si>
+  <si>
+    <t>ֶּ</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>ְ</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>ְּ</t>
+  </si>
+  <si>
+    <t>ַּ</t>
+  </si>
+  <si>
+    <t>ָּ</t>
+  </si>
+  <si>
+    <t>ּׂ</t>
+  </si>
+  <si>
+    <t>ּׁ</t>
+  </si>
+  <si>
+    <t>ֹּ</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>NONE</t>
   </si>
 </sst>
 </file>
@@ -171,9 +252,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,179 +538,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A22" sqref="A1:A1048576"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>

</xml_diff>